<commit_message>
Ajout des sprites animés
</commit_message>
<xml_diff>
--- a/Documents/Dates.xlsx
+++ b/Documents/Dates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT3 Aurora\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacques\Documents\GitHub\SuperStreetMelee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10668"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Sprites attaques basiques</t>
   </si>
@@ -93,14 +93,44 @@
   </si>
   <si>
     <t>Un personnage qui passe hors des limites du terrain se voit ramené avec toute sa vie sur le terrain</t>
+  </si>
+  <si>
+    <t>Gestion de la manette</t>
+  </si>
+  <si>
+    <t>Sprites animés</t>
+  </si>
+  <si>
+    <t>Pour bouger le personnage avec une manette</t>
+  </si>
+  <si>
+    <t>Animations du personnage en idle
+Animation d'une attaque spéciale</t>
+  </si>
+  <si>
+    <t>Pouvoir choisir entre 2 musiques de fond</t>
+  </si>
+  <si>
+    <t>Calendrier Version 6</t>
+  </si>
+  <si>
+    <t>Calendrier Version 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -167,6 +197,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -449,25 +482,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:K19"/>
+  <dimension ref="A6:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
         <v>0</v>
@@ -500,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -531,7 +569,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -566,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -601,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -613,7 +651,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -629,7 +667,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -641,39 +679,128 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>